<commit_message>
finished correct show  dahsboard grafics(#93669)
</commit_message>
<xml_diff>
--- a/data/relatorio_situationx.xlsx
+++ b/data/relatorio_situationx.xlsx
@@ -18,7 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -57,11 +60,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +500,11 @@
           <t>Ativo Atual</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Auditado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -539,6 +548,9 @@
       <c r="M2" t="n">
         <v>501</v>
       </c>
+      <c r="N2" t="n">
+        <v>501</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -552,10 +564,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3" t="n">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E3" t="n">
         <v>18</v>
@@ -584,6 +596,11 @@
       <c r="M3" t="n">
         <v>18</v>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Nenhum</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -649,15 +666,18 @@
           <t>Nenhum</t>
         </is>
       </c>
+      <c r="N4" s="2" t="n">
+        <v>44693.69261477045</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>desvio padrão</t>
+          <t>mínimo</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>259.5011838877074</v>
+        <v>85</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -713,16 +733,19 @@
         <is>
           <t>Nenhum</t>
         </is>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>43834</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>mínimo</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>85</v>
+        <v>335</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -778,16 +801,19 @@
         <is>
           <t>Nenhum</t>
         </is>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>44237</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>mediana</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>335</v>
+        <v>568</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -843,16 +869,19 @@
         <is>
           <t>Nenhum</t>
         </is>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>44679</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>mediana</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>568</v>
+        <v>765</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -908,16 +937,19 @@
         <is>
           <t>Nenhum</t>
         </is>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>45131</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>máximo</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>765</v>
+        <v>999</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -973,16 +1005,19 @@
         <is>
           <t>Nenhum</t>
         </is>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>45656</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>máximo</t>
+          <t>desvio padrão</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>999</v>
+        <v>259.5011838877074</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1035,6 +1070,11 @@
         </is>
       </c>
       <c r="M10" t="inlineStr">
+        <is>
+          <t>Nenhum</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
         <is>
           <t>Nenhum</t>
         </is>
@@ -1074,51 +1114,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CARLA</t>
+          <t>ANA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ANA</t>
+          <t>LETÍCIA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LETÍCIA</t>
+          <t>MARCOS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JOSÉ</t>
+          <t>CARLA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MARCOS</t>
+          <t>JOSÉ</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1159,17 +1199,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FERREIRA S.A</t>
+          <t>DOMINGOS LTDA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -1179,57 +1219,57 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>REZENDE LTDA</t>
+          <t>BARBOSA S.A</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GONÇALVES LTDA</t>
+          <t>FERREIRA S.A</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CARDOSO LTDA</t>
+          <t>GONÇALVES LTDA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BARBOSA S.A</t>
+          <t>REZENDE LTDA</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DOMINGOS LTDA</t>
+          <t>CARDOSO LTDA</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>